<commit_message>
buttons and gliches fixes UI fixes
</commit_message>
<xml_diff>
--- a/db_tables/PlayerScores.xlsx
+++ b/db_tables/PlayerScores.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -54,6 +54,75 @@
   </si>
   <si>
     <t>15000</t>
+  </si>
+  <si>
+    <t>score_1740850946705</t>
+  </si>
+  <si>
+    <t>ofer</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>2025-03-01 19:42:26</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>score_1740852636792</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>2025-03-01 20:10:36</t>
+  </si>
+  <si>
+    <t>5400</t>
+  </si>
+  <si>
+    <t>score_1740851238638</t>
+  </si>
+  <si>
+    <t>oefr</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>2025-03-01 19:47:18</t>
+  </si>
+  <si>
+    <t>4200</t>
+  </si>
+  <si>
+    <t>score_1740851061900</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>2025-03-01 19:44:21</t>
+  </si>
+  <si>
+    <t>2700</t>
+  </si>
+  <si>
+    <t>score_1740852709696</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>2025-03-01 20:11:49</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>30000</t>
   </si>
 </sst>
 </file>
@@ -98,7 +167,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:CV7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -149,6 +218,493 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+      <c r="AP2"/>
+      <c r="AQ2"/>
+      <c r="AR2"/>
+      <c r="AS2"/>
+      <c r="AT2"/>
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
+      <c r="BC2"/>
+      <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2"/>
+      <c r="BG2"/>
+      <c r="BH2"/>
+      <c r="BI2"/>
+      <c r="BJ2"/>
+      <c r="BK2"/>
+      <c r="BL2"/>
+      <c r="BM2"/>
+      <c r="BN2"/>
+      <c r="BO2"/>
+      <c r="BP2"/>
+      <c r="BQ2"/>
+      <c r="BR2"/>
+      <c r="BS2"/>
+      <c r="BT2"/>
+      <c r="BU2"/>
+      <c r="BV2"/>
+      <c r="BW2"/>
+      <c r="BX2"/>
+      <c r="BY2"/>
+      <c r="BZ2"/>
+      <c r="CA2"/>
+      <c r="CB2"/>
+      <c r="CC2"/>
+      <c r="CD2"/>
+      <c r="CE2"/>
+      <c r="CF2"/>
+      <c r="CG2"/>
+      <c r="CH2"/>
+      <c r="CI2"/>
+      <c r="CJ2"/>
+      <c r="CK2"/>
+      <c r="CL2"/>
+      <c r="CM2"/>
+      <c r="CN2"/>
+      <c r="CO2"/>
+      <c r="CP2"/>
+      <c r="CQ2"/>
+      <c r="CR2"/>
+      <c r="CS2"/>
+      <c r="CT2"/>
+      <c r="CU2"/>
+      <c r="CV2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3"/>
+      <c r="AD3"/>
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
+      <c r="AK3"/>
+      <c r="AL3"/>
+      <c r="AM3"/>
+      <c r="AN3"/>
+      <c r="AO3"/>
+      <c r="AP3"/>
+      <c r="AQ3"/>
+      <c r="AR3"/>
+      <c r="AS3"/>
+      <c r="AT3"/>
+      <c r="AU3"/>
+      <c r="AV3"/>
+      <c r="AW3"/>
+      <c r="AX3"/>
+      <c r="AY3"/>
+      <c r="AZ3"/>
+      <c r="BA3"/>
+      <c r="BB3"/>
+      <c r="BC3"/>
+      <c r="BD3"/>
+      <c r="BE3"/>
+      <c r="BF3"/>
+      <c r="BG3"/>
+      <c r="BH3"/>
+      <c r="BI3"/>
+      <c r="BJ3"/>
+      <c r="BK3"/>
+      <c r="BL3"/>
+      <c r="BM3"/>
+      <c r="BN3"/>
+      <c r="BO3"/>
+      <c r="BP3"/>
+      <c r="BQ3"/>
+      <c r="BR3"/>
+      <c r="BS3"/>
+      <c r="BT3"/>
+      <c r="BU3"/>
+      <c r="BV3"/>
+      <c r="BW3"/>
+      <c r="BX3"/>
+      <c r="BY3"/>
+      <c r="BZ3"/>
+      <c r="CA3"/>
+      <c r="CB3"/>
+      <c r="CC3"/>
+      <c r="CD3"/>
+      <c r="CE3"/>
+      <c r="CF3"/>
+      <c r="CG3"/>
+      <c r="CH3"/>
+      <c r="CI3"/>
+      <c r="CJ3"/>
+      <c r="CK3"/>
+      <c r="CL3"/>
+      <c r="CM3"/>
+      <c r="CN3"/>
+      <c r="CO3"/>
+      <c r="CP3"/>
+      <c r="CQ3"/>
+      <c r="CR3"/>
+      <c r="CS3"/>
+      <c r="CT3"/>
+      <c r="CU3"/>
+      <c r="CV3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+      <c r="AB5"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5"/>
+      <c r="AF5"/>
+      <c r="AG5"/>
+      <c r="AH5"/>
+      <c r="AI5"/>
+      <c r="AJ5"/>
+      <c r="AK5"/>
+      <c r="AL5"/>
+      <c r="AM5"/>
+      <c r="AN5"/>
+      <c r="AO5"/>
+      <c r="AP5"/>
+      <c r="AQ5"/>
+      <c r="AR5"/>
+      <c r="AS5"/>
+      <c r="AT5"/>
+      <c r="AU5"/>
+      <c r="AV5"/>
+      <c r="AW5"/>
+      <c r="AX5"/>
+      <c r="AY5"/>
+      <c r="AZ5"/>
+      <c r="BA5"/>
+      <c r="BB5"/>
+      <c r="BC5"/>
+      <c r="BD5"/>
+      <c r="BE5"/>
+      <c r="BF5"/>
+      <c r="BG5"/>
+      <c r="BH5"/>
+      <c r="BI5"/>
+      <c r="BJ5"/>
+      <c r="BK5"/>
+      <c r="BL5"/>
+      <c r="BM5"/>
+      <c r="BN5"/>
+      <c r="BO5"/>
+      <c r="BP5"/>
+      <c r="BQ5"/>
+      <c r="BR5"/>
+      <c r="BS5"/>
+      <c r="BT5"/>
+      <c r="BU5"/>
+      <c r="BV5"/>
+      <c r="BW5"/>
+      <c r="BX5"/>
+      <c r="BY5"/>
+      <c r="BZ5"/>
+      <c r="CA5"/>
+      <c r="CB5"/>
+      <c r="CC5"/>
+      <c r="CD5"/>
+      <c r="CE5"/>
+      <c r="CF5"/>
+      <c r="CG5"/>
+      <c r="CH5"/>
+      <c r="CI5"/>
+      <c r="CJ5"/>
+      <c r="CK5"/>
+      <c r="CL5"/>
+      <c r="CM5"/>
+      <c r="CN5"/>
+      <c r="CO5"/>
+      <c r="CP5"/>
+      <c r="CQ5"/>
+      <c r="CR5"/>
+      <c r="CS5"/>
+      <c r="CT5"/>
+      <c r="CU5"/>
+      <c r="CV5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+      <c r="AB6"/>
+      <c r="AC6"/>
+      <c r="AD6"/>
+      <c r="AE6"/>
+      <c r="AF6"/>
+      <c r="AG6"/>
+      <c r="AH6"/>
+      <c r="AI6"/>
+      <c r="AJ6"/>
+      <c r="AK6"/>
+      <c r="AL6"/>
+      <c r="AM6"/>
+      <c r="AN6"/>
+      <c r="AO6"/>
+      <c r="AP6"/>
+      <c r="AQ6"/>
+      <c r="AR6"/>
+      <c r="AS6"/>
+      <c r="AT6"/>
+      <c r="AU6"/>
+      <c r="AV6"/>
+      <c r="AW6"/>
+      <c r="AX6"/>
+      <c r="AY6"/>
+      <c r="AZ6"/>
+      <c r="BA6"/>
+      <c r="BB6"/>
+      <c r="BC6"/>
+      <c r="BD6"/>
+      <c r="BE6"/>
+      <c r="BF6"/>
+      <c r="BG6"/>
+      <c r="BH6"/>
+      <c r="BI6"/>
+      <c r="BJ6"/>
+      <c r="BK6"/>
+      <c r="BL6"/>
+      <c r="BM6"/>
+      <c r="BN6"/>
+      <c r="BO6"/>
+      <c r="BP6"/>
+      <c r="BQ6"/>
+      <c r="BR6"/>
+      <c r="BS6"/>
+      <c r="BT6"/>
+      <c r="BU6"/>
+      <c r="BV6"/>
+      <c r="BW6"/>
+      <c r="BX6"/>
+      <c r="BY6"/>
+      <c r="BZ6"/>
+      <c r="CA6"/>
+      <c r="CB6"/>
+      <c r="CC6"/>
+      <c r="CD6"/>
+      <c r="CE6"/>
+      <c r="CF6"/>
+      <c r="CG6"/>
+      <c r="CH6"/>
+      <c r="CI6"/>
+      <c r="CJ6"/>
+      <c r="CK6"/>
+      <c r="CL6"/>
+      <c r="CM6"/>
+      <c r="CN6"/>
+      <c r="CO6"/>
+      <c r="CP6"/>
+      <c r="CQ6"/>
+      <c r="CR6"/>
+      <c r="CS6"/>
+      <c r="CT6"/>
+      <c r="CU6"/>
+      <c r="CV6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Add Drill, Pickup, and Drop buttons; adjust HighScoreButton position and aesthetic text
</commit_message>
<xml_diff>
--- a/db_tables/PlayerScores.xlsx
+++ b/db_tables/PlayerScores.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -35,6 +35,90 @@
     <t>TimeRemaining</t>
   </si>
   <si>
+    <t>score_1740851238638</t>
+  </si>
+  <si>
+    <t>oefr</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>2025-03-01 19:47:18</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4200</t>
+  </si>
+  <si>
+    <t>score_1740942082021</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>480</t>
+  </si>
+  <si>
+    <t>EASY</t>
+  </si>
+  <si>
+    <t>2025-03-02 21:01:22</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>50100</t>
+  </si>
+  <si>
+    <t>score_1740850946705</t>
+  </si>
+  <si>
+    <t>ofer</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>2025-03-01 19:42:26</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>score_1740852709696</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>2025-03-01 20:11:49</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>score_1740851061900</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>2025-03-01 19:44:21</t>
+  </si>
+  <si>
+    <t>2700</t>
+  </si>
+  <si>
     <t>score_1740848954723</t>
   </si>
   <si>
@@ -44,33 +128,12 @@
     <t>350</t>
   </si>
   <si>
-    <t>MEDIUM</t>
-  </si>
-  <si>
     <t>2025-03-01 19:09:14</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>15000</t>
   </si>
   <si>
-    <t>score_1740850946705</t>
-  </si>
-  <si>
-    <t>ofer</t>
-  </si>
-  <si>
-    <t>320</t>
-  </si>
-  <si>
-    <t>2025-03-01 19:42:26</t>
-  </si>
-  <si>
-    <t>12000</t>
-  </si>
-  <si>
     <t>score_1740852636792</t>
   </si>
   <si>
@@ -81,48 +144,6 @@
   </si>
   <si>
     <t>5400</t>
-  </si>
-  <si>
-    <t>score_1740851238638</t>
-  </si>
-  <si>
-    <t>oefr</t>
-  </si>
-  <si>
-    <t>240</t>
-  </si>
-  <si>
-    <t>2025-03-01 19:47:18</t>
-  </si>
-  <si>
-    <t>4200</t>
-  </si>
-  <si>
-    <t>score_1740851061900</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>2025-03-01 19:44:21</t>
-  </si>
-  <si>
-    <t>2700</t>
-  </si>
-  <si>
-    <t>score_1740852709696</t>
-  </si>
-  <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>2025-03-01 20:11:49</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>30000</t>
   </si>
 </sst>
 </file>
@@ -167,7 +188,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:CV7"/>
+  <dimension ref="A1:CV8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -323,155 +344,155 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="Y3"/>
-      <c r="Z3"/>
-      <c r="AA3"/>
-      <c r="AB3"/>
-      <c r="AC3"/>
-      <c r="AD3"/>
-      <c r="AE3"/>
-      <c r="AF3"/>
-      <c r="AG3"/>
-      <c r="AH3"/>
-      <c r="AI3"/>
-      <c r="AJ3"/>
-      <c r="AK3"/>
-      <c r="AL3"/>
-      <c r="AM3"/>
-      <c r="AN3"/>
-      <c r="AO3"/>
-      <c r="AP3"/>
-      <c r="AQ3"/>
-      <c r="AR3"/>
-      <c r="AS3"/>
-      <c r="AT3"/>
-      <c r="AU3"/>
-      <c r="AV3"/>
-      <c r="AW3"/>
-      <c r="AX3"/>
-      <c r="AY3"/>
-      <c r="AZ3"/>
-      <c r="BA3"/>
-      <c r="BB3"/>
-      <c r="BC3"/>
-      <c r="BD3"/>
-      <c r="BE3"/>
-      <c r="BF3"/>
-      <c r="BG3"/>
-      <c r="BH3"/>
-      <c r="BI3"/>
-      <c r="BJ3"/>
-      <c r="BK3"/>
-      <c r="BL3"/>
-      <c r="BM3"/>
-      <c r="BN3"/>
-      <c r="BO3"/>
-      <c r="BP3"/>
-      <c r="BQ3"/>
-      <c r="BR3"/>
-      <c r="BS3"/>
-      <c r="BT3"/>
-      <c r="BU3"/>
-      <c r="BV3"/>
-      <c r="BW3"/>
-      <c r="BX3"/>
-      <c r="BY3"/>
-      <c r="BZ3"/>
-      <c r="CA3"/>
-      <c r="CB3"/>
-      <c r="CC3"/>
-      <c r="CD3"/>
-      <c r="CE3"/>
-      <c r="CF3"/>
-      <c r="CG3"/>
-      <c r="CH3"/>
-      <c r="CI3"/>
-      <c r="CJ3"/>
-      <c r="CK3"/>
-      <c r="CL3"/>
-      <c r="CM3"/>
-      <c r="CN3"/>
-      <c r="CO3"/>
-      <c r="CP3"/>
-      <c r="CQ3"/>
-      <c r="CR3"/>
-      <c r="CS3"/>
-      <c r="CT3"/>
-      <c r="CU3"/>
-      <c r="CV3"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AG4"/>
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AJ4"/>
+      <c r="AK4"/>
+      <c r="AL4"/>
+      <c r="AM4"/>
+      <c r="AN4"/>
+      <c r="AO4"/>
+      <c r="AP4"/>
+      <c r="AQ4"/>
+      <c r="AR4"/>
+      <c r="AS4"/>
+      <c r="AT4"/>
+      <c r="AU4"/>
+      <c r="AV4"/>
+      <c r="AW4"/>
+      <c r="AX4"/>
+      <c r="AY4"/>
+      <c r="AZ4"/>
+      <c r="BA4"/>
+      <c r="BB4"/>
+      <c r="BC4"/>
+      <c r="BD4"/>
+      <c r="BE4"/>
+      <c r="BF4"/>
+      <c r="BG4"/>
+      <c r="BH4"/>
+      <c r="BI4"/>
+      <c r="BJ4"/>
+      <c r="BK4"/>
+      <c r="BL4"/>
+      <c r="BM4"/>
+      <c r="BN4"/>
+      <c r="BO4"/>
+      <c r="BP4"/>
+      <c r="BQ4"/>
+      <c r="BR4"/>
+      <c r="BS4"/>
+      <c r="BT4"/>
+      <c r="BU4"/>
+      <c r="BV4"/>
+      <c r="BW4"/>
+      <c r="BX4"/>
+      <c r="BY4"/>
+      <c r="BZ4"/>
+      <c r="CA4"/>
+      <c r="CB4"/>
+      <c r="CC4"/>
+      <c r="CD4"/>
+      <c r="CE4"/>
+      <c r="CF4"/>
+      <c r="CG4"/>
+      <c r="CH4"/>
+      <c r="CI4"/>
+      <c r="CJ4"/>
+      <c r="CK4"/>
+      <c r="CL4"/>
+      <c r="CM4"/>
+      <c r="CN4"/>
+      <c r="CO4"/>
+      <c r="CP4"/>
+      <c r="CQ4"/>
+      <c r="CR4"/>
+      <c r="CS4"/>
+      <c r="CT4"/>
+      <c r="CU4"/>
+      <c r="CV4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -569,25 +590,25 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -685,26 +706,235 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+      <c r="AA7"/>
+      <c r="AB7"/>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7"/>
+      <c r="AF7"/>
+      <c r="AG7"/>
+      <c r="AH7"/>
+      <c r="AI7"/>
+      <c r="AJ7"/>
+      <c r="AK7"/>
+      <c r="AL7"/>
+      <c r="AM7"/>
+      <c r="AN7"/>
+      <c r="AO7"/>
+      <c r="AP7"/>
+      <c r="AQ7"/>
+      <c r="AR7"/>
+      <c r="AS7"/>
+      <c r="AT7"/>
+      <c r="AU7"/>
+      <c r="AV7"/>
+      <c r="AW7"/>
+      <c r="AX7"/>
+      <c r="AY7"/>
+      <c r="AZ7"/>
+      <c r="BA7"/>
+      <c r="BB7"/>
+      <c r="BC7"/>
+      <c r="BD7"/>
+      <c r="BE7"/>
+      <c r="BF7"/>
+      <c r="BG7"/>
+      <c r="BH7"/>
+      <c r="BI7"/>
+      <c r="BJ7"/>
+      <c r="BK7"/>
+      <c r="BL7"/>
+      <c r="BM7"/>
+      <c r="BN7"/>
+      <c r="BO7"/>
+      <c r="BP7"/>
+      <c r="BQ7"/>
+      <c r="BR7"/>
+      <c r="BS7"/>
+      <c r="BT7"/>
+      <c r="BU7"/>
+      <c r="BV7"/>
+      <c r="BW7"/>
+      <c r="BX7"/>
+      <c r="BY7"/>
+      <c r="BZ7"/>
+      <c r="CA7"/>
+      <c r="CB7"/>
+      <c r="CC7"/>
+      <c r="CD7"/>
+      <c r="CE7"/>
+      <c r="CF7"/>
+      <c r="CG7"/>
+      <c r="CH7"/>
+      <c r="CI7"/>
+      <c r="CJ7"/>
+      <c r="CK7"/>
+      <c r="CL7"/>
+      <c r="CM7"/>
+      <c r="CN7"/>
+      <c r="CO7"/>
+      <c r="CP7"/>
+      <c r="CQ7"/>
+      <c r="CR7"/>
+      <c r="CS7"/>
+      <c r="CT7"/>
+      <c r="CU7"/>
+      <c r="CV7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
+      <c r="AK8"/>
+      <c r="AL8"/>
+      <c r="AM8"/>
+      <c r="AN8"/>
+      <c r="AO8"/>
+      <c r="AP8"/>
+      <c r="AQ8"/>
+      <c r="AR8"/>
+      <c r="AS8"/>
+      <c r="AT8"/>
+      <c r="AU8"/>
+      <c r="AV8"/>
+      <c r="AW8"/>
+      <c r="AX8"/>
+      <c r="AY8"/>
+      <c r="AZ8"/>
+      <c r="BA8"/>
+      <c r="BB8"/>
+      <c r="BC8"/>
+      <c r="BD8"/>
+      <c r="BE8"/>
+      <c r="BF8"/>
+      <c r="BG8"/>
+      <c r="BH8"/>
+      <c r="BI8"/>
+      <c r="BJ8"/>
+      <c r="BK8"/>
+      <c r="BL8"/>
+      <c r="BM8"/>
+      <c r="BN8"/>
+      <c r="BO8"/>
+      <c r="BP8"/>
+      <c r="BQ8"/>
+      <c r="BR8"/>
+      <c r="BS8"/>
+      <c r="BT8"/>
+      <c r="BU8"/>
+      <c r="BV8"/>
+      <c r="BW8"/>
+      <c r="BX8"/>
+      <c r="BY8"/>
+      <c r="BZ8"/>
+      <c r="CA8"/>
+      <c r="CB8"/>
+      <c r="CC8"/>
+      <c r="CD8"/>
+      <c r="CE8"/>
+      <c r="CF8"/>
+      <c r="CG8"/>
+      <c r="CH8"/>
+      <c r="CI8"/>
+      <c r="CJ8"/>
+      <c r="CK8"/>
+      <c r="CL8"/>
+      <c r="CM8"/>
+      <c r="CN8"/>
+      <c r="CO8"/>
+      <c r="CP8"/>
+      <c r="CQ8"/>
+      <c r="CR8"/>
+      <c r="CS8"/>
+      <c r="CT8"/>
+      <c r="CU8"/>
+      <c r="CV8"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>